<commit_message>
added documentation to code
</commit_message>
<xml_diff>
--- a/src/hw1/code/data_from_code.xlsx
+++ b/src/hw1/code/data_from_code.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -91,6 +91,22 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,14 +129,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5063,7 +5095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B14:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="113" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScale="113" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -5287,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A10:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="F14" zoomScale="94" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>

</xml_diff>